<commit_message>
assets [img] [json] [xslx] - under license
</commit_message>
<xml_diff>
--- a/assets/json/sncf.xlsx
+++ b/assets/json/sncf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbouy\VSCode\VSCodeWorkspace\flutter\galapsbs\assets\json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21726750-B221-49FA-BE76-436FCF168DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A4B922-8CCC-47A5-AEAC-D800E850C42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="350">
   <si>
     <t>Julie</t>
   </si>
@@ -336,9 +336,6 @@
     <t>Margaux</t>
   </si>
   <si>
-    <t>Hatt</t>
-  </si>
-  <si>
     <t>Lucas</t>
   </si>
   <si>
@@ -1072,6 +1069,12 @@
   </si>
   <si>
     <t>Labonne</t>
+  </si>
+  <si>
+    <t>Briac</t>
+  </si>
+  <si>
+    <t>Morice</t>
   </si>
 </sst>
 </file>
@@ -1424,8 +1427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
-      <selection activeCell="D242" sqref="D242"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2525,10 +2528,10 @@
         <v>9</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>102</v>
+        <v>348</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>103</v>
+        <v>349</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -2545,10 +2548,10 @@
         <v>9</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>11</v>
@@ -2575,7 +2578,7 @@
         <v>5</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>2</v>
@@ -2592,10 +2595,10 @@
         <v>10</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>2</v>
@@ -2612,10 +2615,10 @@
         <v>10</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>2</v>
@@ -2632,10 +2635,10 @@
         <v>10</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>2</v>
@@ -2652,10 +2655,10 @@
         <v>10</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>2</v>
@@ -2672,10 +2675,10 @@
         <v>10</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>2</v>
@@ -2699,10 +2702,10 @@
         <v>11</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>2</v>
@@ -2719,10 +2722,10 @@
         <v>11</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>2</v>
@@ -2739,10 +2742,10 @@
         <v>11</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>2</v>
@@ -2759,10 +2762,10 @@
         <v>11</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>2</v>
@@ -2779,10 +2782,10 @@
         <v>11</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>2</v>
@@ -2799,10 +2802,10 @@
         <v>11</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>2</v>
@@ -2826,10 +2829,10 @@
         <v>12</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>2</v>
@@ -2846,10 +2849,10 @@
         <v>12</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>2</v>
@@ -2866,10 +2869,10 @@
         <v>12</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>2</v>
@@ -2886,10 +2889,10 @@
         <v>12</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>11</v>
@@ -2906,10 +2909,10 @@
         <v>12</v>
       </c>
       <c r="B82" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>2</v>
@@ -2926,11 +2929,11 @@
         <v>12</v>
       </c>
       <c r="B83" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="D83" s="1" t="s">
         <v>11</v>
       </c>
@@ -2938,7 +2941,7 @@
         <v>3</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2953,10 +2956,10 @@
         <v>13</v>
       </c>
       <c r="B85" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>2</v>
@@ -2973,10 +2976,10 @@
         <v>13</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>2</v>
@@ -2993,10 +2996,10 @@
         <v>13</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>2</v>
@@ -3013,10 +3016,10 @@
         <v>13</v>
       </c>
       <c r="B88" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>2</v>
@@ -3033,10 +3036,10 @@
         <v>13</v>
       </c>
       <c r="B89" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>2</v>
@@ -3053,10 +3056,10 @@
         <v>13</v>
       </c>
       <c r="B90" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C90" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>2</v>
@@ -3080,10 +3083,10 @@
         <v>14</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>2</v>
@@ -3100,10 +3103,10 @@
         <v>14</v>
       </c>
       <c r="B93" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>2</v>
@@ -3123,7 +3126,7 @@
         <v>46</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>11</v>
@@ -3140,10 +3143,10 @@
         <v>14</v>
       </c>
       <c r="B95" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>2</v>
@@ -3160,10 +3163,10 @@
         <v>14</v>
       </c>
       <c r="B96" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>2</v>
@@ -3183,7 +3186,7 @@
         <v>20</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>2</v>
@@ -3207,10 +3210,10 @@
         <v>15</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>11</v>
@@ -3227,10 +3230,10 @@
         <v>15</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>11</v>
@@ -3247,10 +3250,10 @@
         <v>15</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>2</v>
@@ -3267,10 +3270,10 @@
         <v>15</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -3287,10 +3290,10 @@
         <v>15</v>
       </c>
       <c r="B103" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>2</v>
@@ -3307,10 +3310,10 @@
         <v>15</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -3334,10 +3337,10 @@
         <v>16</v>
       </c>
       <c r="B106" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>11</v>
@@ -3354,10 +3357,10 @@
         <v>16</v>
       </c>
       <c r="B107" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>2</v>
@@ -3374,10 +3377,10 @@
         <v>16</v>
       </c>
       <c r="B108" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>2</v>
@@ -3397,7 +3400,7 @@
         <v>40</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>2</v>
@@ -3417,7 +3420,7 @@
         <v>54</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -3434,10 +3437,10 @@
         <v>16</v>
       </c>
       <c r="B111" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>2</v>
@@ -3461,10 +3464,10 @@
         <v>17</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>11</v>
@@ -3481,10 +3484,10 @@
         <v>17</v>
       </c>
       <c r="B114" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C114" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>2</v>
@@ -3501,10 +3504,10 @@
         <v>17</v>
       </c>
       <c r="B115" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>2</v>
@@ -3521,10 +3524,10 @@
         <v>17</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -3544,7 +3547,7 @@
         <v>30</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>11</v>
@@ -3561,10 +3564,10 @@
         <v>17</v>
       </c>
       <c r="B118" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>11</v>
@@ -3588,10 +3591,10 @@
         <v>18</v>
       </c>
       <c r="B120" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>2</v>
@@ -3608,10 +3611,10 @@
         <v>18</v>
       </c>
       <c r="B121" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>11</v>
@@ -3628,10 +3631,10 @@
         <v>18</v>
       </c>
       <c r="B122" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>2</v>
@@ -3651,7 +3654,7 @@
         <v>12</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>2</v>
@@ -3668,10 +3671,10 @@
         <v>18</v>
       </c>
       <c r="B124" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C124" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>2</v>
@@ -3688,10 +3691,10 @@
         <v>18</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>11</v>
@@ -3715,10 +3718,10 @@
         <v>19</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>2</v>
@@ -3735,10 +3738,10 @@
         <v>19</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>2</v>
@@ -3758,7 +3761,7 @@
         <v>22</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>2</v>
@@ -3775,10 +3778,10 @@
         <v>19</v>
       </c>
       <c r="B130" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C130" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>2</v>
@@ -3795,10 +3798,10 @@
         <v>19</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>11</v>
@@ -3818,7 +3821,7 @@
         <v>22</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>11</v>
@@ -3845,7 +3848,7 @@
         <v>5</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>2</v>
@@ -3862,10 +3865,10 @@
         <v>20</v>
       </c>
       <c r="B135" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C135" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>2</v>
@@ -3882,10 +3885,10 @@
         <v>20</v>
       </c>
       <c r="B136" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C136" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>215</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>11</v>
@@ -3902,10 +3905,10 @@
         <v>20</v>
       </c>
       <c r="B137" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C137" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>2</v>
@@ -3925,7 +3928,7 @@
         <v>24</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D138" s="1" t="s">
         <v>11</v>
@@ -3942,10 +3945,10 @@
         <v>20</v>
       </c>
       <c r="B139" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C139" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>11</v>
@@ -3969,10 +3972,10 @@
         <v>21</v>
       </c>
       <c r="B141" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C141" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>2</v>
@@ -3992,7 +3995,7 @@
         <v>9</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>2</v>
@@ -4012,7 +4015,7 @@
         <v>78</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>2</v>
@@ -4029,10 +4032,10 @@
         <v>21</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>2</v>
@@ -4049,10 +4052,10 @@
         <v>21</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>11</v>
@@ -4069,10 +4072,10 @@
         <v>21</v>
       </c>
       <c r="B146" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C146" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>2</v>
@@ -4096,10 +4099,10 @@
         <v>22</v>
       </c>
       <c r="B148" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C148" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>2</v>
@@ -4119,7 +4122,7 @@
         <v>86</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>2</v>
@@ -4136,10 +4139,10 @@
         <v>22</v>
       </c>
       <c r="B150" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C150" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>11</v>
@@ -4156,10 +4159,10 @@
         <v>22</v>
       </c>
       <c r="B151" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C151" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>2</v>
@@ -4179,7 +4182,7 @@
         <v>0</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>11</v>
@@ -4199,7 +4202,7 @@
         <v>12</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>2</v>
@@ -4223,10 +4226,10 @@
         <v>23</v>
       </c>
       <c r="B155" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C155" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>2</v>
@@ -4243,10 +4246,10 @@
         <v>23</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>2</v>
@@ -4266,7 +4269,7 @@
         <v>102</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D157" s="1" t="s">
         <v>11</v>
@@ -4283,10 +4286,10 @@
         <v>23</v>
       </c>
       <c r="B158" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C158" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>2</v>
@@ -4303,10 +4306,10 @@
         <v>23</v>
       </c>
       <c r="B159" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C159" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>11</v>
@@ -4323,10 +4326,10 @@
         <v>23</v>
       </c>
       <c r="B160" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C160" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>2</v>
@@ -4353,7 +4356,7 @@
         <v>84</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D162" s="1" t="s">
         <v>11</v>
@@ -4370,10 +4373,10 @@
         <v>24</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>11</v>
@@ -4390,10 +4393,10 @@
         <v>24</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D164" s="1" t="s">
         <v>11</v>
@@ -4410,10 +4413,10 @@
         <v>24</v>
       </c>
       <c r="B165" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C165" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>251</v>
       </c>
       <c r="D165" s="1" t="s">
         <v>11</v>
@@ -4430,10 +4433,10 @@
         <v>24</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>2</v>
@@ -4453,7 +4456,7 @@
         <v>32</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D167" s="1" t="s">
         <v>2</v>
@@ -4480,7 +4483,7 @@
         <v>92</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D169" s="1" t="s">
         <v>11</v>
@@ -4497,10 +4500,10 @@
         <v>25</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D170" s="1" t="s">
         <v>11</v>
@@ -4517,10 +4520,10 @@
         <v>25</v>
       </c>
       <c r="B171" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C171" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>257</v>
       </c>
       <c r="D171" s="1" t="s">
         <v>2</v>
@@ -4537,10 +4540,10 @@
         <v>25</v>
       </c>
       <c r="B172" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C172" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>259</v>
       </c>
       <c r="D172" s="1" t="s">
         <v>2</v>
@@ -4557,16 +4560,16 @@
         <v>25</v>
       </c>
       <c r="B173" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C173" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C173" s="1" t="s">
+      <c r="D173" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E173" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="D173" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>4</v>
@@ -4577,10 +4580,10 @@
         <v>25</v>
       </c>
       <c r="B174" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C174" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>264</v>
       </c>
       <c r="D174" s="1" t="s">
         <v>2</v>
@@ -4604,10 +4607,10 @@
         <v>26</v>
       </c>
       <c r="B176" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C176" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="C176" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>2</v>
@@ -4624,10 +4627,10 @@
         <v>26</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D177" s="1" t="s">
         <v>11</v>
@@ -4644,16 +4647,16 @@
         <v>26</v>
       </c>
       <c r="B178" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C178" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="C178" s="1" t="s">
-        <v>269</v>
-      </c>
       <c r="D178" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>4</v>
@@ -4664,10 +4667,10 @@
         <v>26</v>
       </c>
       <c r="B179" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C179" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="C179" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="D179" s="1" t="s">
         <v>2</v>
@@ -4684,10 +4687,10 @@
         <v>26</v>
       </c>
       <c r="B180" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C180" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="C180" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>11</v>
@@ -4707,7 +4710,7 @@
         <v>40</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>2</v>
@@ -4734,7 +4737,7 @@
         <v>100</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D183" s="1" t="s">
         <v>2</v>
@@ -4751,16 +4754,16 @@
         <v>27</v>
       </c>
       <c r="B184" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C184" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C184" s="1" t="s">
-        <v>277</v>
-      </c>
       <c r="D184" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>4</v>
@@ -4771,10 +4774,10 @@
         <v>27</v>
       </c>
       <c r="B185" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C185" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="C185" s="1" t="s">
-        <v>279</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>11</v>
@@ -4791,10 +4794,10 @@
         <v>27</v>
       </c>
       <c r="B186" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C186" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="C186" s="1" t="s">
-        <v>281</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>2</v>
@@ -4814,13 +4817,13 @@
         <v>9</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D187" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>4</v>
@@ -4831,10 +4834,10 @@
         <v>27</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>2</v>
@@ -4861,7 +4864,7 @@
         <v>9</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>11</v>
@@ -4878,10 +4881,10 @@
         <v>28</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D191" s="1" t="s">
         <v>11</v>
@@ -4898,10 +4901,10 @@
         <v>28</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D192" s="1" t="s">
         <v>11</v>
@@ -4921,7 +4924,7 @@
         <v>86</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D193" s="1" t="s">
         <v>2</v>
@@ -4938,10 +4941,10 @@
         <v>28</v>
       </c>
       <c r="B194" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C194" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="C194" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="D194" s="1" t="s">
         <v>2</v>
@@ -4958,10 +4961,10 @@
         <v>28</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D195" s="1" t="s">
         <v>2</v>
@@ -4985,10 +4988,10 @@
         <v>29</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D197" s="1" t="s">
         <v>11</v>
@@ -5005,16 +5008,16 @@
         <v>29</v>
       </c>
       <c r="B198" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C198" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="C198" s="1" t="s">
-        <v>292</v>
-      </c>
       <c r="D198" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>17</v>
@@ -5028,7 +5031,7 @@
         <v>67</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D199" s="1" t="s">
         <v>2</v>
@@ -5045,10 +5048,10 @@
         <v>29</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D200" s="1" t="s">
         <v>2</v>
@@ -5065,10 +5068,10 @@
         <v>29</v>
       </c>
       <c r="B201" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C201" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="C201" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="D201" s="1" t="s">
         <v>2</v>
@@ -5088,7 +5091,7 @@
         <v>24</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D202" s="1" t="s">
         <v>2</v>
@@ -5112,10 +5115,10 @@
         <v>30</v>
       </c>
       <c r="B204" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C204" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="C204" s="1" t="s">
-        <v>299</v>
       </c>
       <c r="D204" s="1" t="s">
         <v>11</v>
@@ -5135,7 +5138,7 @@
         <v>20</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D205" s="1" t="s">
         <v>2</v>
@@ -5152,10 +5155,10 @@
         <v>30</v>
       </c>
       <c r="B206" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C206" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="C206" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="D206" s="1" t="s">
         <v>11</v>
@@ -5172,10 +5175,10 @@
         <v>30</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D207" s="1" t="s">
         <v>2</v>
@@ -5192,10 +5195,10 @@
         <v>30</v>
       </c>
       <c r="B208" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C208" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="C208" s="1" t="s">
-        <v>305</v>
       </c>
       <c r="D208" s="1" t="s">
         <v>11</v>
@@ -5212,10 +5215,10 @@
         <v>30</v>
       </c>
       <c r="B209" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C209" s="1" t="s">
         <v>306</v>
-      </c>
-      <c r="C209" s="1" t="s">
-        <v>307</v>
       </c>
       <c r="D209" s="1" t="s">
         <v>11</v>
@@ -5242,7 +5245,7 @@
         <v>32</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D211" s="1" t="s">
         <v>2</v>
@@ -5259,10 +5262,10 @@
         <v>31</v>
       </c>
       <c r="B212" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C212" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="C212" s="1" t="s">
-        <v>310</v>
       </c>
       <c r="D212" s="1" t="s">
         <v>11</v>
@@ -5279,16 +5282,16 @@
         <v>31</v>
       </c>
       <c r="B213" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C213" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="C213" s="1" t="s">
-        <v>312</v>
-      </c>
       <c r="D213" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>4</v>
@@ -5299,10 +5302,10 @@
         <v>31</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D214" s="1" t="s">
         <v>2</v>
@@ -5319,10 +5322,10 @@
         <v>31</v>
       </c>
       <c r="B215" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C215" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="C215" s="1" t="s">
-        <v>315</v>
       </c>
       <c r="D215" s="1" t="s">
         <v>11</v>
@@ -5339,10 +5342,10 @@
         <v>31</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D216" s="1" t="s">
         <v>11</v>
@@ -5366,10 +5369,10 @@
         <v>32</v>
       </c>
       <c r="B218" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C218" s="1" t="s">
         <v>317</v>
-      </c>
-      <c r="C218" s="1" t="s">
-        <v>318</v>
       </c>
       <c r="D218" s="1" t="s">
         <v>2</v>
@@ -5386,10 +5389,10 @@
         <v>32</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D219" s="1" t="s">
         <v>11</v>
@@ -5406,10 +5409,10 @@
         <v>32</v>
       </c>
       <c r="B220" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C220" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="C220" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="D220" s="1" t="s">
         <v>2</v>
@@ -5426,10 +5429,10 @@
         <v>32</v>
       </c>
       <c r="B221" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C221" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="C221" s="1" t="s">
-        <v>323</v>
       </c>
       <c r="D221" s="1" t="s">
         <v>11</v>
@@ -5446,10 +5449,10 @@
         <v>32</v>
       </c>
       <c r="B222" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C222" s="1" t="s">
         <v>324</v>
-      </c>
-      <c r="C222" s="1" t="s">
-        <v>325</v>
       </c>
       <c r="D222" s="1" t="s">
         <v>2</v>
@@ -5466,10 +5469,10 @@
         <v>32</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D223" s="1" t="s">
         <v>11</v>
@@ -5493,10 +5496,10 @@
         <v>33</v>
       </c>
       <c r="B225" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C225" s="1" t="s">
         <v>327</v>
-      </c>
-      <c r="C225" s="1" t="s">
-        <v>328</v>
       </c>
       <c r="D225" s="1" t="s">
         <v>11</v>
@@ -5513,10 +5516,10 @@
         <v>33</v>
       </c>
       <c r="B226" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C226" s="1" t="s">
         <v>329</v>
-      </c>
-      <c r="C226" s="1" t="s">
-        <v>330</v>
       </c>
       <c r="D226" s="1" t="s">
         <v>11</v>
@@ -5533,19 +5536,19 @@
         <v>33</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C227" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D227" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="D227" s="1" t="s">
+      <c r="E227" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F227" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="E227" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="F227" s="1" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="228" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5553,16 +5556,16 @@
         <v>33</v>
       </c>
       <c r="B228" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C228" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="C228" s="1" t="s">
-        <v>334</v>
-      </c>
       <c r="D228" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F228" s="1" t="s">
         <v>4</v>
@@ -5573,10 +5576,10 @@
         <v>33</v>
       </c>
       <c r="B229" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C229" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="C229" s="1" t="s">
-        <v>336</v>
       </c>
       <c r="D229" s="1" t="s">
         <v>2</v>
@@ -5593,16 +5596,16 @@
         <v>33</v>
       </c>
       <c r="B230" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C230" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="C230" s="1" t="s">
-        <v>338</v>
-      </c>
       <c r="D230" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F230" s="1" t="s">
         <v>17</v>
@@ -5620,10 +5623,10 @@
         <v>34</v>
       </c>
       <c r="B232" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C232" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="C232" s="1" t="s">
-        <v>340</v>
       </c>
       <c r="D232" s="1" t="s">
         <v>2</v>
@@ -5640,10 +5643,10 @@
         <v>34</v>
       </c>
       <c r="B233" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C233" s="1" t="s">
         <v>341</v>
-      </c>
-      <c r="C233" s="1" t="s">
-        <v>342</v>
       </c>
       <c r="D233" s="1" t="s">
         <v>11</v>
@@ -5660,16 +5663,16 @@
         <v>34</v>
       </c>
       <c r="B234" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C234" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C234" s="1" t="s">
-        <v>344</v>
-      </c>
       <c r="D234" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F234" s="1" t="s">
         <v>17</v>
@@ -5680,16 +5683,16 @@
         <v>34</v>
       </c>
       <c r="B235" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C235" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="C235" s="1" t="s">
-        <v>346</v>
-      </c>
       <c r="D235" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F235" s="1" t="s">
         <v>17</v>
@@ -5700,10 +5703,10 @@
         <v>34</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D236" s="1" t="s">
         <v>11</v>
@@ -5723,7 +5726,7 @@
         <v>62</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D237" s="1" t="s">
         <v>11</v>

</xml_diff>